<commit_message>
Al gusto del nigga
Ok?
</commit_message>
<xml_diff>
--- a/masters.xlsx
+++ b/masters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aitorjara/Documents/GitHub/machine_learning_shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713F6FBD-CD34-584C-89FB-9BBF8A5EC9D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC2B212-D9B9-4147-A83A-3025291FFFB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="440" windowWidth="23840" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,7 +552,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
   <si>
     <t>Title</t>
   </si>
@@ -804,6 +804,9 @@
   </si>
   <si>
     <t>IGOR</t>
+  </si>
+  <si>
+    <t>AITOR</t>
   </si>
 </sst>
 </file>
@@ -899,7 +902,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -909,18 +912,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2B6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -939,7 +930,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -948,10 +939,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -964,6 +952,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF77FF90"/>
+      <color rgb="FFFF6866"/>
       <color rgb="FFFFF2B6"/>
     </mruColors>
   </colors>
@@ -1301,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1365,6 +1355,9 @@
       <c r="D2" t="s">
         <v>34</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
@@ -1397,6 +1390,9 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F3" t="s">
         <v>38</v>
       </c>
@@ -1426,6 +1422,9 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F4" t="s">
         <v>38</v>
       </c>
@@ -1455,6 +1454,9 @@
       <c r="D5" t="s">
         <v>34</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F5" t="s">
         <v>35</v>
       </c>
@@ -1484,7 +1486,9 @@
       <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
       <c r="F6" t="s">
         <v>40</v>
       </c>
@@ -1514,7 +1518,7 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>83</v>
       </c>
       <c r="F7" t="s">
@@ -1546,7 +1550,7 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>83</v>
       </c>
       <c r="F8" t="s">
@@ -1578,7 +1582,9 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
       <c r="F9" t="s">
         <v>33</v>
       </c>
@@ -1608,7 +1614,9 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
@@ -1638,7 +1646,9 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
@@ -1668,7 +1678,9 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F12" t="s">
         <v>51</v>
       </c>
@@ -1698,7 +1710,9 @@
       <c r="D13" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F13" t="s">
         <v>81</v>
       </c>
@@ -1728,7 +1742,9 @@
       <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F14" t="s">
         <v>60</v>
       </c>
@@ -1758,7 +1774,9 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F15" t="s">
         <v>63</v>
       </c>
@@ -1788,7 +1806,9 @@
       <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F16" t="s">
         <v>66</v>
       </c>
@@ -1821,7 +1841,9 @@
       <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F17" t="s">
         <v>71</v>
       </c>
@@ -1854,7 +1876,9 @@
       <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F18" t="s">
         <v>63</v>
       </c>
@@ -1887,7 +1911,9 @@
       <c r="D19" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="F19" t="s">
         <v>77</v>
       </c>
@@ -1913,6 +1939,16 @@
       <sortCondition ref="A1:A9"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="E2:E19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF6866"/>
+        <color rgb="FF77FF90"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>